<commit_message>
New stage test 0630
</commit_message>
<xml_diff>
--- a/tech_log.xlsx
+++ b/tech_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy\Downloads\G-eternal\G-Eternal Hard Stage Database\G-Eternal Hard Stage Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3CAEA2-BAE1-4786-814D-9132D6218139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19966F95-BFF5-4352-9FF7-E39B0A6E2F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3088B17-E40C-4C57-948D-AD84F438F619}"/>
+    <workbookView xWindow="16815" yWindow="2325" windowWidth="10635" windowHeight="11295" xr2:uid="{E3088B17-E40C-4C57-948D-AD84F438F619}"/>
   </bookViews>
   <sheets>
     <sheet name="tech_log" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,6 +611,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -774,8 +780,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1178,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF4961F-D97D-4E03-89BC-73996B9D8EC0}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,76 +1207,76 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>12-D2*3-C2</f>
-        <v>-5</v>
+        <v>-11</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
         <f>E2+3*F2</f>
-        <v>-2</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E43" si="0">12-D3*3-C3</f>
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G43" si="1">E3+3*F3</f>
-        <v>4</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="H4">
         <f>SUMIF(G2:G4,"&gt;0")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1324,72 +1331,72 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-9</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="H9">
         <f>SUMIF(G7:G9,"&gt;0")</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1400,18 +1407,18 @@
         <v>19</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-13</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1422,21 +1429,21 @@
         <v>21</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1447,21 +1454,21 @@
         <v>23</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>-28</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1472,25 +1479,25 @@
         <v>25</v>
       </c>
       <c r="C13">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>-18</v>
+        <v>-35</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>-15</v>
+        <v>-32</v>
       </c>
       <c r="H13">
         <f>SUMIF(G10:G13,"&gt;0")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1501,18 +1508,18 @@
         <v>27</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1523,21 +1530,21 @@
         <v>29</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-11</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1548,101 +1555,101 @@
         <v>31</v>
       </c>
       <c r="C16">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-13</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="H16">
         <f>SUMIF(G14:G16,"&gt;0")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C17">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-12</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-11</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-11</v>
       </c>
       <c r="H19">
         <f>SUMIF(G17:G19,"&gt;0")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1653,21 +1660,21 @@
         <v>39</v>
       </c>
       <c r="C20">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>4</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>-14</v>
+        <v>-37</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>-11</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1678,21 +1685,21 @@
         <v>41</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-16</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1703,21 +1710,21 @@
         <v>43</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D22">
         <v>4</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-22</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1728,18 +1735,18 @@
         <v>45</v>
       </c>
       <c r="C23">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>-14</v>
+        <v>-34</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>-14</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1750,18 +1757,18 @@
         <v>47</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-11</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1775,15 +1782,15 @@
         <v>9</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="H25">
         <f>SUMIF(G20:G25,"&gt;0")</f>
@@ -1798,21 +1805,21 @@
         <v>51</v>
       </c>
       <c r="C26">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-33</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1823,21 +1830,21 @@
         <v>53</v>
       </c>
       <c r="C27">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D27">
         <v>4</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-30</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1848,18 +1855,18 @@
         <v>55</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1870,18 +1877,18 @@
         <v>57</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1892,25 +1899,25 @@
         <v>59</v>
       </c>
       <c r="C30">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-15</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-12</v>
       </c>
       <c r="H30">
         <f>SUMIF(G26:G30,"&gt;0")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1921,21 +1928,21 @@
         <v>61</v>
       </c>
       <c r="C31">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1949,44 +1956,44 @@
         <v>11</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-8</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>64</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C33">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-10</v>
       </c>
       <c r="H33">
         <f>SUMIF(G31:G33,"&gt;0")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1997,18 +2004,18 @@
         <v>67</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-13</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2019,21 +2026,21 @@
         <v>69</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2044,18 +2051,18 @@
         <v>71</v>
       </c>
       <c r="C36">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D36">
         <v>4</v>
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-33</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>-10</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2066,21 +2073,21 @@
         <v>73</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-11</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2091,25 +2098,25 @@
         <v>75</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="H38">
         <f>SUMIF(G34:G38,"&gt;0")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2120,21 +2127,21 @@
         <v>77</v>
       </c>
       <c r="C39">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D39">
         <v>4</v>
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>-29</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39">
         <f t="shared" si="1"/>
-        <v>-8</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2145,21 +2152,21 @@
         <v>79</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2170,18 +2177,18 @@
         <v>81</v>
       </c>
       <c r="C41">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-11</v>
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2192,18 +2199,18 @@
         <v>83</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="G42">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2214,25 +2221,25 @@
         <v>85</v>
       </c>
       <c r="C43">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D43">
         <v>4</v>
       </c>
       <c r="E43">
         <f t="shared" si="0"/>
-        <v>-16</v>
+        <v>-40</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43">
         <f t="shared" si="1"/>
-        <v>-13</v>
+        <v>-37</v>
       </c>
       <c r="H43">
         <f>SUMIF(G39:G43,"&gt;0")</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>